<commit_message>
order id filter added for custom order admin script
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/ManageProducts/ManageProducts.xlsx
+++ b/binaries/FCfiles/ManageProducts/ManageProducts.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="115">
   <si>
     <t>Other</t>
   </si>
@@ -367,6 +367,9 @@
   </si>
   <si>
     <t>prodUlWZ</t>
+  </si>
+  <si>
+    <t>prodvBwQ</t>
   </si>
 </sst>
 </file>
@@ -397,7 +400,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="148">
+  <fills count="150">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1134,8 +1137,18 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="152">
+  <borders count="154">
     <border>
       <left/>
       <right/>
@@ -1820,11 +1833,18 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="94">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0">
@@ -1945,7 +1965,8 @@
     <xf applyBorder="true" applyFill="true" borderId="145" fillId="141" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="147" fillId="143" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="149" fillId="145" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="147" borderId="151" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="151" fillId="147" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="149" borderId="153" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -2447,8 +2468,8 @@
       <c r="A5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="85" t="s">
-        <v>106</v>
+      <c r="B5" s="93" t="s">
+        <v>114</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Scripts updated as per failures
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/ManageProducts/ManageProducts.xlsx
+++ b/binaries/FCfiles/ManageProducts/ManageProducts.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="138">
   <si>
     <t>Other</t>
   </si>
@@ -388,6 +388,57 @@
   </si>
   <si>
     <t>prodQjpg</t>
+  </si>
+  <si>
+    <t>prodUBTd</t>
+  </si>
+  <si>
+    <t>prodRRAG</t>
+  </si>
+  <si>
+    <t>prodxPOB</t>
+  </si>
+  <si>
+    <t>prodAEhD</t>
+  </si>
+  <si>
+    <t>prodGTCg</t>
+  </si>
+  <si>
+    <t>prodbYUG</t>
+  </si>
+  <si>
+    <t>prodhjwH</t>
+  </si>
+  <si>
+    <t>prodrlpt</t>
+  </si>
+  <si>
+    <t>prodwTYJ</t>
+  </si>
+  <si>
+    <t>prodZEcH</t>
+  </si>
+  <si>
+    <t>prodPYZo</t>
+  </si>
+  <si>
+    <t>prodmFfn</t>
+  </si>
+  <si>
+    <t>prodpdMX</t>
+  </si>
+  <si>
+    <t>prodTvcZ</t>
+  </si>
+  <si>
+    <t>prodKSUp</t>
+  </si>
+  <si>
+    <t>prodQROt</t>
+  </si>
+  <si>
+    <t>prodtJdk</t>
   </si>
 </sst>
 </file>
@@ -418,7 +469,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="162">
+  <fills count="196">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1225,8 +1276,178 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="166">
+  <borders count="200">
     <border>
       <left/>
       <right/>
@@ -1960,11 +2181,130 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="117">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0">
@@ -2092,7 +2432,24 @@
     <xf applyBorder="true" applyFill="true" borderId="159" fillId="155" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="161" fillId="157" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="163" fillId="159" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="161" borderId="165" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="165" fillId="161" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="167" fillId="163" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="169" fillId="165" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="171" fillId="167" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="173" fillId="169" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="175" fillId="171" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="177" fillId="173" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="179" fillId="175" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="181" fillId="177" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="183" fillId="179" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="185" fillId="181" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="187" fillId="183" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="189" fillId="185" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="191" fillId="187" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="193" fillId="189" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="195" fillId="191" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="197" fillId="193" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="195" borderId="199" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -2462,8 +2819,8 @@
       <c r="A2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="99" t="s">
-        <v>120</v>
+      <c r="B2" s="116" t="s">
+        <v>137</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>17</v>
@@ -2500,8 +2857,8 @@
       <c r="A3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="92" t="s">
-        <v>113</v>
+      <c r="B3" s="110" t="s">
+        <v>131</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>17</v>
@@ -2594,8 +2951,8 @@
       <c r="A5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="93" t="s">
-        <v>114</v>
+      <c r="B5" s="111" t="s">
+        <v>132</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>17</v>

</xml_diff>